<commit_message>
laporan inventaris + barcode
</commit_message>
<xml_diff>
--- a/public/files/template/inventory/kibinventaris.xlsx
+++ b/public/files/template/inventory/kibinventaris.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t>Buku Invetaris</t>
   </si>
@@ -141,6 +141,27 @@
   </si>
   <si>
     <t>[b.kd_kab]</t>
+  </si>
+  <si>
+    <t>[a.pilihan_asal]</t>
+  </si>
+  <si>
+    <t>[a.keterangan_pengadaan]</t>
+  </si>
+  <si>
+    <t>[a.merk]</t>
+  </si>
+  <si>
+    <t>[a.nobukti]</t>
+  </si>
+  <si>
+    <t>[a.bahan]</t>
+  </si>
+  <si>
+    <t>[a.ukuran]</t>
+  </si>
+  <si>
+    <t>[a.satuan]</t>
   </si>
 </sst>
 </file>
@@ -237,10 +258,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -525,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -605,26 +626,26 @@
       </c>
     </row>
     <row r="12" spans="1:15" ht="15.75">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7" t="s">
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
-      <c r="M12" s="7" t="s">
+      <c r="M12" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="N12" s="7"/>
+      <c r="N12" s="8"/>
       <c r="O12" s="3"/>
     </row>
     <row r="13" spans="1:15" ht="63">
@@ -722,7 +743,7 @@
       </c>
     </row>
     <row r="15" spans="1:15">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B15" s="6" t="s">
@@ -734,15 +755,27 @@
       <c r="D15" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
+      <c r="E15" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>39</v>
+      </c>
       <c r="I15" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
+      <c r="J15" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>45</v>
+      </c>
       <c r="L15" s="6" t="s">
         <v>36</v>
       </c>
@@ -752,7 +785,9 @@
       <c r="N15" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="O15" s="6"/>
+      <c r="O15" s="6" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>